<commit_message>
added brent and inflation data
</commit_message>
<xml_diff>
--- a/output/tables/results/Results ArCo.xlsx
+++ b/output/tables/results/Results ArCo.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c98b824bff33be6/MSc. Econometrics VU/MSc. Econometrics Year 2/MSc. Thesis/Coding/msc_thesis_v3/output/tables/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{5DCC0CE6-C424-4DDE-8CC3-14B354F52E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E645CE36-888E-44F2-94C6-13FADAADD003}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{5DCC0CE6-C424-4DDE-8CC3-14B354F52E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C6BE58C-0055-4680-85B5-062E094B57B7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{141255E8-19F8-4AA2-BE3F-1547732D56A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="France" sheetId="1" r:id="rId1"/>
-    <sheet name="United Kingdom" sheetId="2" r:id="rId2"/>
-    <sheet name="Switzerland" sheetId="3" r:id="rId3"/>
-    <sheet name="Ireland" sheetId="4" r:id="rId4"/>
-    <sheet name="Portugal" sheetId="5" r:id="rId5"/>
+    <sheet name="All" sheetId="6" r:id="rId1"/>
+    <sheet name="France" sheetId="1" r:id="rId2"/>
+    <sheet name="United Kingdom" sheetId="2" r:id="rId3"/>
+    <sheet name="Switzerland" sheetId="3" r:id="rId4"/>
+    <sheet name="Ireland" sheetId="4" r:id="rId5"/>
+    <sheet name="Portugal" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
   <si>
     <t>CO2</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t># Relevant regressors</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Impl year</t>
   </si>
 </sst>
 </file>
@@ -111,9 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -130,6 +150,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,11 +452,190 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A099A1DC-9A1D-41C1-AF7E-1A525046E7A3}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="7" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2008</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2013</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.71420993769154695</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.28032716707806299</v>
+      </c>
+      <c r="E3">
+        <v>0.67753526202034997</v>
+      </c>
+      <c r="F3">
+        <v>0.125771940734308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2E-3</v>
+      </c>
+      <c r="E4">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>72</v>
+      </c>
+      <c r="C7">
+        <v>96</v>
+      </c>
+      <c r="D7">
+        <v>132</v>
+      </c>
+      <c r="E7">
+        <v>144</v>
+      </c>
+      <c r="F7">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>142</v>
+      </c>
+      <c r="C8">
+        <v>118</v>
+      </c>
+      <c r="D8">
+        <v>82</v>
+      </c>
+      <c r="E8">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8601DD13-869A-4B9D-9C91-C069D386E1BD}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,19 +745,19 @@
       <c r="B5">
         <v>0.65495732606660095</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <v>0.669123212148241</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>0.65314546299467702</v>
       </c>
     </row>
@@ -678,7 +881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE89ACB2-EF68-4FD6-BB6D-87E39B31C58D}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -793,16 +996,16 @@
       <c r="B5">
         <v>0.47185273973499098</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <v>0.61649176049590004</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
@@ -816,16 +1019,16 @@
       <c r="B6">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
@@ -929,7 +1132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E7424D-4ED6-4335-9C25-ABBECBF48879}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -1044,16 +1247,16 @@
       <c r="B5">
         <v>0.72009798535918701</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
@@ -1067,16 +1270,16 @@
       <c r="B6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
@@ -1090,16 +1293,16 @@
       <c r="B7">
         <v>11</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>9</v>
       </c>
       <c r="G7">
@@ -1113,16 +1316,16 @@
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
@@ -1180,7 +1383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26167306-CFF4-412F-8977-761C2ADE491D}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -1431,7 +1634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0942BD4-9428-4195-A335-4337457CA36D}">
   <dimension ref="A1:G10"/>
   <sheetViews>

</xml_diff>